<commit_message>
Compartmentalized each part of script.py by writing the steps as functions in naics.py, and calling them in the new script.py. There are many style changes as well.  Functionally, the script now creates an naics tree with FA, INV, LAND for each sector--finishing the section 2.2 in the documentation, which was hopefully one of the most difficult parts.
</commit_message>
<xml_diff>
--- a/Data/Calibration/DepreciationParameters/Program/data/SOI_Partner/Crosswalks/12pa01_Crosswalk.xlsx
+++ b/Data/Calibration/DepreciationParameters/Program/data/SOI_Partner/Crosswalks/12pa01_Crosswalk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>All industries</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>31.32.33</t>
+  </si>
+  <si>
+    <t>Other real estate activities</t>
+  </si>
+  <si>
+    <t>5313</t>
   </si>
 </sst>
 </file>
@@ -787,9 +793,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1558,321 +1566,329 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="3">
-        <v>532</v>
+        <v>143</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" s="3">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" s="3">
-        <v>54</v>
+        <v>533</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" s="3">
-        <v>5411</v>
+        <v>54</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" s="3">
-        <v>5412</v>
+        <v>5411</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" s="3">
-        <v>5413</v>
+        <v>5412</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" s="3">
-        <v>5414</v>
+        <v>5413</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" s="3">
-        <v>5415</v>
+        <v>5414</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" s="3">
-        <v>5416</v>
+        <v>5415</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" s="3">
-        <v>5418</v>
+        <v>5416</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" s="3">
-        <v>5419</v>
+        <v>5418</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" s="3">
-        <v>55</v>
+        <v>5419</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" s="3">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" s="3">
-        <v>561</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" s="3">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" s="3">
-        <v>61</v>
+        <v>562</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>140</v>
+        <v>110</v>
+      </c>
+      <c r="B113" s="3">
+        <v>62</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B114" s="3">
-        <v>6213</v>
+        <v>111</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" s="3">
-        <v>6214</v>
+        <v>6213</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" s="3">
-        <v>6215</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" s="3">
-        <v>6216</v>
+        <v>6215</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" s="3">
-        <v>6219</v>
+        <v>6216</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" s="3">
-        <v>622</v>
+        <v>6219</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" s="3">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" s="3">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" s="3">
-        <v>71</v>
+        <v>624</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="3">
-        <v>711</v>
+        <v>71</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" s="3">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" s="3">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" s="3">
-        <v>72</v>
+        <v>713</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" s="3">
-        <v>721</v>
+        <v>72</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" s="3">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" s="3">
-        <v>81</v>
+        <v>722</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" s="3">
-        <v>811</v>
+        <v>81</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" s="3">
-        <v>8111</v>
+        <v>811</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
+      </c>
+      <c r="B132" s="3">
+        <v>8111</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B133" s="3">
-        <v>812</v>
+        <v>130</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="3">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B135" s="3">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B135" s="2"/>
+      <c r="B136" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>